<commit_message>
updated news and teams
</commit_message>
<xml_diff>
--- a/teams-and-rosters/CS320-Sp19-Teams.xlsx
+++ b/teams-and-rosters/CS320-Sp19-Teams.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\djhake2\cs320-spring2019\teams-and-rosters\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="90" windowWidth="12570" windowHeight="12075"/>
   </bookViews>
@@ -274,7 +279,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -284,12 +289,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -401,7 +400,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -446,18 +445,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -549,7 +536,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -584,7 +571,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -796,7 +783,7 @@
   <dimension ref="B2:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -809,12 +796,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="F2" s="9"/>
     </row>
     <row r="3" spans="2:6" ht="26.25" x14ac:dyDescent="0.4">
@@ -825,21 +812,21 @@
       <c r="F3" s="7"/>
     </row>
     <row r="4" spans="2:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="2:6" s="5" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
       <c r="F5" s="8"/>
     </row>
     <row r="6" spans="2:6" s="2" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -860,10 +847,10 @@
       <c r="B7" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="17" t="s">
         <v>32</v>
       </c>
       <c r="E7" s="10" t="s">
@@ -874,10 +861,10 @@
       <c r="B8" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="18" t="s">
         <v>36</v>
       </c>
       <c r="E8" s="11" t="s">
@@ -888,10 +875,10 @@
       <c r="B9" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="D9" s="19" t="s">
         <v>43</v>
       </c>
       <c r="E9" s="12" t="s">
@@ -899,32 +886,32 @@
       </c>
     </row>
     <row r="10" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="24"/>
+      <c r="D10" s="20"/>
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="2:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="2:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
       <c r="F12" s="6"/>
     </row>
     <row r="13" spans="2:6" s="5" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="2:6" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -942,72 +929,72 @@
       </c>
     </row>
     <row r="15" spans="2:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="21" t="s">
+      <c r="D15" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="21" t="s">
+      <c r="E15" s="17" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="D16" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="22" t="s">
+      <c r="E16" s="18" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="23" t="s">
+      <c r="C17" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="23" t="s">
+      <c r="D17" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="23" t="s">
+      <c r="E17" s="19" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="25" t="s">
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="21" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="19" spans="2:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="2:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="B20" s="30" t="s">
+      <c r="B20" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="30"/>
-      <c r="D20" s="30"/>
-      <c r="E20" s="30"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
       <c r="F20" s="6"/>
     </row>
     <row r="21" spans="2:6" s="5" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="29" t="s">
+      <c r="B21" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="29"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
       <c r="F21" s="4"/>
     </row>
     <row r="22" spans="2:6" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1031,10 +1018,10 @@
       <c r="C23" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="27" t="s">
+      <c r="D23" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="E23" s="27" t="s">
+      <c r="E23" s="23" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1045,10 +1032,10 @@
       <c r="C24" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D24" s="22" t="s">
+      <c r="D24" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="E24" s="22" t="s">
+      <c r="E24" s="18" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1059,10 +1046,10 @@
       <c r="C25" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D25" s="22" t="s">
+      <c r="D25" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="E25" s="22" t="s">
+      <c r="E25" s="18" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1071,8 +1058,8 @@
         <v>9</v>
       </c>
       <c r="C26" s="14"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
     </row>
     <row r="27" spans="2:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>

</xml_diff>